<commit_message>
Change Assignment 2 Self Evaluation
</commit_message>
<xml_diff>
--- a/Topical Assignment 2/Assignment 02 Self Evaluation.xlsx
+++ b/Topical Assignment 2/Assignment 02 Self Evaluation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA01600-C5BA-4299-9C19-D46163337751}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A7FADB-A3CF-407C-9B1A-040D4C2AD93C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4500" yWindow="4365" windowWidth="25155" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 05" sheetId="1" r:id="rId1"/>
@@ -1729,18 +1729,6 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1762,6 +1750,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2080,55 +2080,57 @@
   <sheetPr codeName="shtAssignment05"/>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="44" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="100.7109375" customWidth="1"/>
-    <col min="8" max="8" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.73046875" customWidth="1"/>
+    <col min="2" max="2" width="64.265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.73046875" style="44" customWidth="1"/>
+    <col min="4" max="4" width="15.73046875" customWidth="1"/>
+    <col min="5" max="5" width="12.73046875" customWidth="1"/>
+    <col min="6" max="6" width="10.73046875" customWidth="1"/>
+    <col min="7" max="7" width="100.73046875" customWidth="1"/>
+    <col min="8" max="8" width="50.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9"/>
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="37"/>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="74" t="s">
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="73" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="11"/>
       <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="38"/>
-      <c r="D2" s="68"/>
+      <c r="D2" s="68">
+        <v>3</v>
+      </c>
       <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="13"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="78"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="71"/>
+      <c r="H2" s="74"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>10</v>
@@ -2139,10 +2141,10 @@
         <v>5</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="78"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="71"/>
+      <c r="H3" s="74"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>11</v>
@@ -2153,10 +2155,10 @@
         <v>5</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="79"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="72"/>
+      <c r="H4" s="75"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="38"/>
@@ -2166,7 +2168,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="29"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="38" t="s">
@@ -2186,7 +2188,7 @@
       </c>
       <c r="H6" s="30"/>
     </row>
-    <row r="7" spans="1:8" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="31"/>
       <c r="B7" s="32" t="s">
         <v>1</v>
@@ -2205,8 +2207,8 @@
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="71" t="s">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="76" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -2214,20 +2216,20 @@
       </c>
       <c r="C8" s="40"/>
       <c r="D8" s="18" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E8" s="19">
         <v>5</v>
       </c>
       <c r="F8" s="19">
         <f t="shared" ref="F8:F36" si="0">IF(D8="No",-E8,0)</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="70"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="77"/>
       <c r="B9" s="12" t="s">
         <v>17</v>
       </c>
@@ -2235,20 +2237,20 @@
         <v>13</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E9" s="23">
         <v>5</v>
       </c>
       <c r="F9" s="23">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G9" s="24"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="70"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="77"/>
       <c r="B10" s="12" t="s">
         <v>107</v>
       </c>
@@ -2256,20 +2258,20 @@
         <v>14</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E10" s="23">
         <v>5</v>
       </c>
       <c r="F10" s="23">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="70"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="77"/>
       <c r="B11" s="12" t="s">
         <v>18</v>
       </c>
@@ -2277,20 +2279,20 @@
         <v>15</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E11" s="23">
         <v>5</v>
       </c>
       <c r="F11" s="23">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G11" s="24"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="72"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="78"/>
       <c r="B12" s="12" t="s">
         <v>19</v>
       </c>
@@ -2298,20 +2300,20 @@
         <v>16</v>
       </c>
       <c r="D12" s="48" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E12" s="49">
         <v>5</v>
       </c>
       <c r="F12" s="49">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="69" t="s">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="79" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="25" t="s">
@@ -2321,20 +2323,20 @@
         <v>20</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E13" s="27">
         <v>3</v>
       </c>
       <c r="F13" s="27">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="70"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="77"/>
       <c r="B14" s="21" t="s">
         <v>33</v>
       </c>
@@ -2342,20 +2344,20 @@
         <v>34</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E14" s="23">
         <v>3</v>
       </c>
       <c r="F14" s="23">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="70"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="77"/>
       <c r="B15" s="21" t="s">
         <v>59</v>
       </c>
@@ -2363,20 +2365,20 @@
         <v>60</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E15" s="23">
         <v>3</v>
       </c>
       <c r="F15" s="23">
         <f t="shared" ref="F15" si="1">IF(D15="No",-E15,0)</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="70"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="77"/>
       <c r="B16" s="21" t="s">
         <v>61</v>
       </c>
@@ -2384,20 +2386,20 @@
         <v>62</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E16" s="23">
         <v>3</v>
       </c>
       <c r="F16" s="23">
         <f t="shared" ref="F16" si="2">IF(D16="No",-E16,0)</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="70"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="77"/>
       <c r="B17" s="21" t="s">
         <v>47</v>
       </c>
@@ -2405,20 +2407,20 @@
         <v>69</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E17" s="23">
         <v>3</v>
       </c>
       <c r="F17" s="23">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="70"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="77"/>
       <c r="B18" s="21" t="s">
         <v>45</v>
       </c>
@@ -2426,20 +2428,20 @@
         <v>66</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E18" s="23">
         <v>3</v>
       </c>
       <c r="F18" s="23">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="70"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="77"/>
       <c r="B19" s="21" t="s">
         <v>48</v>
       </c>
@@ -2447,20 +2449,20 @@
         <v>66</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E19" s="23">
         <v>3</v>
       </c>
       <c r="F19" s="23">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="70"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="77"/>
       <c r="B20" s="21" t="s">
         <v>49</v>
       </c>
@@ -2468,20 +2470,20 @@
         <v>66</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E20" s="23">
         <v>3</v>
       </c>
       <c r="F20" s="23">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="70"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="77"/>
       <c r="B21" s="21" t="s">
         <v>46</v>
       </c>
@@ -2489,20 +2491,20 @@
         <v>68</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E21" s="23">
         <v>3</v>
       </c>
       <c r="F21" s="23">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="70"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="77"/>
       <c r="B22" s="21" t="s">
         <v>50</v>
       </c>
@@ -2510,20 +2512,20 @@
         <v>68</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E22" s="23">
         <v>3</v>
       </c>
       <c r="F22" s="23">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="70"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="77"/>
       <c r="B23" s="21" t="s">
         <v>49</v>
       </c>
@@ -2531,20 +2533,20 @@
         <v>68</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E23" s="23">
         <v>3</v>
       </c>
       <c r="F23" s="23">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="70"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="77"/>
       <c r="B24" s="21" t="s">
         <v>51</v>
       </c>
@@ -2552,20 +2554,20 @@
         <v>67</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E24" s="23">
         <v>3</v>
       </c>
       <c r="F24" s="23">
         <f t="shared" ref="F24:F28" si="3">IF(D24="No",-E24,0)</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="70"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="77"/>
       <c r="B25" s="21" t="s">
         <v>48</v>
       </c>
@@ -2573,20 +2575,20 @@
         <v>67</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E25" s="23">
         <v>3</v>
       </c>
       <c r="F25" s="23">
         <f t="shared" si="3"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="70"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="77"/>
       <c r="B26" s="21" t="s">
         <v>49</v>
       </c>
@@ -2594,20 +2596,20 @@
         <v>67</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E26" s="23">
         <v>3</v>
       </c>
       <c r="F26" s="23">
         <f t="shared" si="3"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="70"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" s="77"/>
       <c r="B27" s="21" t="s">
         <v>52</v>
       </c>
@@ -2615,20 +2617,20 @@
         <v>63</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E27" s="23">
         <v>3</v>
       </c>
       <c r="F27" s="23">
         <f t="shared" si="3"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="70"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" s="77"/>
       <c r="B28" s="21" t="s">
         <v>54</v>
       </c>
@@ -2636,20 +2638,20 @@
         <v>63</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E28" s="23">
         <v>3</v>
       </c>
       <c r="F28" s="23">
         <f t="shared" si="3"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="70"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" s="77"/>
       <c r="B29" s="21" t="s">
         <v>53</v>
       </c>
@@ -2657,20 +2659,20 @@
         <v>63</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E29" s="23">
         <v>3</v>
       </c>
       <c r="F29" s="23">
         <f t="shared" ref="F29" si="4">IF(D29="No",-E29,0)</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G29" s="54"/>
       <c r="H29" s="24"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="72"/>
+    <row r="30" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A30" s="78"/>
       <c r="B30" s="21" t="s">
         <v>64</v>
       </c>
@@ -2678,20 +2680,20 @@
         <v>65</v>
       </c>
       <c r="D30" s="45" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E30" s="46">
         <v>3</v>
       </c>
       <c r="F30" s="46">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G30" s="47"/>
       <c r="H30" s="24"/>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="69" t="s">
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="79" t="s">
         <v>25</v>
       </c>
       <c r="B31" s="25" t="s">
@@ -2701,20 +2703,20 @@
         <v>36</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E31" s="27">
         <v>3</v>
       </c>
       <c r="F31" s="27">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G31" s="28"/>
       <c r="H31" s="20"/>
     </row>
-    <row r="32" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="70"/>
+    <row r="32" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A32" s="77"/>
       <c r="B32" s="21" t="s">
         <v>55</v>
       </c>
@@ -2722,20 +2724,20 @@
         <v>70</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E32" s="23">
         <v>3</v>
       </c>
       <c r="F32" s="23">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G32" s="24"/>
       <c r="H32" s="24"/>
     </row>
-    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="70"/>
+    <row r="33" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A33" s="77"/>
       <c r="B33" s="21" t="s">
         <v>56</v>
       </c>
@@ -2755,8 +2757,8 @@
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
     </row>
-    <row r="34" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="70"/>
+    <row r="34" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A34" s="77"/>
       <c r="B34" s="21" t="s">
         <v>57</v>
       </c>
@@ -2776,8 +2778,8 @@
       <c r="G34" s="24"/>
       <c r="H34" s="24"/>
     </row>
-    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="70"/>
+    <row r="35" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A35" s="77"/>
       <c r="B35" s="21" t="s">
         <v>58</v>
       </c>
@@ -2797,8 +2799,8 @@
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="70"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" s="77"/>
       <c r="B36" s="50" t="s">
         <v>37</v>
       </c>
@@ -2816,7 +2818,7 @@
       <c r="G36" s="54"/>
       <c r="H36" s="54"/>
     </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="55" t="s">
         <v>38</v>
       </c>
@@ -2828,13 +2830,13 @@
       <c r="E37" s="59"/>
       <c r="F37" s="59">
         <f>MAX(-35,SUM(F8:F36))</f>
-        <v>-35</v>
+        <v>-14</v>
       </c>
       <c r="G37" s="60"/>
       <c r="H37" s="60"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="71" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" s="76" t="s">
         <v>26</v>
       </c>
       <c r="B38" s="17" t="s">
@@ -2854,8 +2856,8 @@
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="70"/>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A39" s="77"/>
       <c r="B39" s="12" t="s">
         <v>17</v>
       </c>
@@ -2875,8 +2877,8 @@
       <c r="G39" s="24"/>
       <c r="H39" s="16"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="70"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A40" s="77"/>
       <c r="B40" s="12" t="s">
         <v>107</v>
       </c>
@@ -2896,8 +2898,8 @@
       <c r="G40" s="24"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="70"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A41" s="77"/>
       <c r="B41" s="12" t="s">
         <v>18</v>
       </c>
@@ -2917,8 +2919,8 @@
       <c r="G41" s="24"/>
       <c r="H41" s="16"/>
     </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="72"/>
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="78"/>
       <c r="B42" s="12" t="s">
         <v>19</v>
       </c>
@@ -2938,8 +2940,8 @@
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="69" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A43" s="79" t="s">
         <v>27</v>
       </c>
       <c r="B43" s="25" t="s">
@@ -2961,8 +2963,8 @@
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="70"/>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A44" s="77"/>
       <c r="B44" s="65" t="s">
         <v>83</v>
       </c>
@@ -2982,8 +2984,8 @@
       <c r="G44" s="67"/>
       <c r="H44" s="67"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="70"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A45" s="77"/>
       <c r="B45" s="21" t="s">
         <v>42</v>
       </c>
@@ -3003,8 +3005,8 @@
       <c r="G45" s="24"/>
       <c r="H45" s="24"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="70"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A46" s="77"/>
       <c r="B46" s="21" t="s">
         <v>71</v>
       </c>
@@ -3024,8 +3026,8 @@
       <c r="G46" s="24"/>
       <c r="H46" s="24"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="70"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A47" s="77"/>
       <c r="B47" s="21" t="s">
         <v>74</v>
       </c>
@@ -3045,8 +3047,8 @@
       <c r="G47" s="24"/>
       <c r="H47" s="24"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="70"/>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A48" s="77"/>
       <c r="B48" s="21" t="s">
         <v>75</v>
       </c>
@@ -3066,8 +3068,8 @@
       <c r="G48" s="24"/>
       <c r="H48" s="24"/>
     </row>
-    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="70"/>
+    <row r="49" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A49" s="77"/>
       <c r="B49" s="21" t="s">
         <v>77</v>
       </c>
@@ -3087,8 +3089,8 @@
       <c r="G49" s="24"/>
       <c r="H49" s="24"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="70"/>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A50" s="77"/>
       <c r="B50" s="21" t="s">
         <v>78</v>
       </c>
@@ -3108,8 +3110,8 @@
       <c r="G50" s="24"/>
       <c r="H50" s="24"/>
     </row>
-    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="70"/>
+    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="77"/>
       <c r="B51" s="50" t="s">
         <v>80</v>
       </c>
@@ -3129,7 +3131,7 @@
       <c r="G51" s="54"/>
       <c r="H51" s="54"/>
     </row>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A52" s="55" t="s">
         <v>38</v>
       </c>
@@ -3146,8 +3148,8 @@
       <c r="G52" s="60"/>
       <c r="H52" s="60"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="71" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A53" s="76" t="s">
         <v>28</v>
       </c>
       <c r="B53" s="17" t="s">
@@ -3167,8 +3169,8 @@
       <c r="G53" s="20"/>
       <c r="H53" s="20"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="70"/>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A54" s="77"/>
       <c r="B54" s="12" t="s">
         <v>17</v>
       </c>
@@ -3188,8 +3190,8 @@
       <c r="G54" s="24"/>
       <c r="H54" s="16"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="70"/>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A55" s="77"/>
       <c r="B55" s="12" t="s">
         <v>107</v>
       </c>
@@ -3209,8 +3211,8 @@
       <c r="G55" s="24"/>
       <c r="H55" s="16"/>
     </row>
-    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="70"/>
+    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="77"/>
       <c r="B56" s="12" t="s">
         <v>18</v>
       </c>
@@ -3230,8 +3232,8 @@
       <c r="G56" s="24"/>
       <c r="H56" s="16"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="72"/>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A57" s="78"/>
       <c r="B57" s="12" t="s">
         <v>19</v>
       </c>
@@ -3251,8 +3253,8 @@
       <c r="G57" s="16"/>
       <c r="H57" s="16"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="69" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A58" s="79" t="s">
         <v>29</v>
       </c>
       <c r="B58" s="25" t="s">
@@ -3274,8 +3276,8 @@
       <c r="G58" s="28"/>
       <c r="H58" s="28"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="70"/>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A59" s="77"/>
       <c r="B59" s="65" t="s">
         <v>82</v>
       </c>
@@ -3295,8 +3297,8 @@
       <c r="G59" s="67"/>
       <c r="H59" s="67"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="70"/>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A60" s="77"/>
       <c r="B60" s="21" t="s">
         <v>84</v>
       </c>
@@ -3316,8 +3318,8 @@
       <c r="G60" s="24"/>
       <c r="H60" s="24"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="70"/>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A61" s="77"/>
       <c r="B61" s="64" t="s">
         <v>89</v>
       </c>
@@ -3337,8 +3339,8 @@
       <c r="G61" s="24"/>
       <c r="H61" s="24"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="70"/>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A62" s="77"/>
       <c r="B62" s="64" t="s">
         <v>90</v>
       </c>
@@ -3358,8 +3360,8 @@
       <c r="G62" s="24"/>
       <c r="H62" s="24"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="70"/>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A63" s="77"/>
       <c r="B63" s="21" t="s">
         <v>87</v>
       </c>
@@ -3379,8 +3381,8 @@
       <c r="G63" s="24"/>
       <c r="H63" s="24"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="70"/>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A64" s="77"/>
       <c r="B64" s="21" t="s">
         <v>88</v>
       </c>
@@ -3400,8 +3402,8 @@
       <c r="G64" s="24"/>
       <c r="H64" s="24"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="70"/>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A65" s="77"/>
       <c r="B65" s="21" t="s">
         <v>92</v>
       </c>
@@ -3421,8 +3423,8 @@
       <c r="G65" s="24"/>
       <c r="H65" s="24"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="70"/>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A66" s="77"/>
       <c r="B66" s="21" t="s">
         <v>93</v>
       </c>
@@ -3442,8 +3444,8 @@
       <c r="G66" s="24"/>
       <c r="H66" s="24"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="70"/>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A67" s="77"/>
       <c r="B67" s="21" t="s">
         <v>94</v>
       </c>
@@ -3463,8 +3465,8 @@
       <c r="G67" s="24"/>
       <c r="H67" s="24"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="70"/>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A68" s="77"/>
       <c r="B68" s="64" t="s">
         <v>96</v>
       </c>
@@ -3484,8 +3486,8 @@
       <c r="G68" s="24"/>
       <c r="H68" s="24"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="70"/>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A69" s="77"/>
       <c r="B69" s="64" t="s">
         <v>97</v>
       </c>
@@ -3505,8 +3507,8 @@
       <c r="G69" s="24"/>
       <c r="H69" s="24"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="70"/>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A70" s="77"/>
       <c r="B70" s="21" t="s">
         <v>99</v>
       </c>
@@ -3526,8 +3528,8 @@
       <c r="G70" s="24"/>
       <c r="H70" s="24"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="70"/>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A71" s="77"/>
       <c r="B71" s="21" t="s">
         <v>100</v>
       </c>
@@ -3547,8 +3549,8 @@
       <c r="G71" s="24"/>
       <c r="H71" s="24"/>
     </row>
-    <row r="72" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A72" s="70"/>
+    <row r="72" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A72" s="77"/>
       <c r="B72" s="21" t="s">
         <v>101</v>
       </c>
@@ -3568,8 +3570,8 @@
       <c r="G72" s="24"/>
       <c r="H72" s="24"/>
     </row>
-    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="70"/>
+    <row r="73" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A73" s="77"/>
       <c r="B73" s="21" t="s">
         <v>102</v>
       </c>
@@ -3589,8 +3591,8 @@
       <c r="G73" s="24"/>
       <c r="H73" s="24"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="70"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A74" s="77"/>
       <c r="B74" s="50" t="s">
         <v>104</v>
       </c>
@@ -3610,7 +3612,7 @@
       <c r="G74" s="54"/>
       <c r="H74" s="54"/>
     </row>
-    <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A75" s="55" t="s">
         <v>38</v>
       </c>
@@ -3627,12 +3629,12 @@
       <c r="G75" s="60"/>
       <c r="H75" s="60"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="1"/>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77" s="2"/>
       <c r="B77" s="61" t="s">
         <v>4</v>
@@ -3642,12 +3644,12 @@
       <c r="E77" s="63"/>
       <c r="F77" s="63">
         <f>MAX(-99,F7+F37+F52+F75)</f>
-        <v>-95</v>
+        <v>-74</v>
       </c>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
     </row>
-    <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A78" s="3"/>
       <c r="B78" s="7" t="s">
         <v>30</v>
@@ -3657,7 +3659,7 @@
       <c r="E78" s="4"/>
       <c r="F78" s="4">
         <f>100+F77</f>
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="G78" s="6"/>
       <c r="H78" s="6"/>
@@ -3665,16 +3667,16 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="1Wy2qOxqzvlJZwC15VrqVUfgXri5CXyDLw8J9g9wUgLPNUERQeHFkBwl3BUP6E7QDvz410JUTtv4F78JJNxIXg==" saltValue="vMQlgNidT+i49dELMM/ijg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="10">
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A43:A51"/>
+    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="A58:A74"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:G4"/>
     <mergeCell ref="H1:H4"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A30"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A43:A51"/>
-    <mergeCell ref="A53:A57"/>
-    <mergeCell ref="A58:A74"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{0C4A7BFB-837E-4FE4-8988-52705A9B035E}">

</xml_diff>

<commit_message>
Add Extension Method and Tests to Master Project
</commit_message>
<xml_diff>
--- a/Topical Assignment 2/Assignment 02 Self Evaluation.xlsx
+++ b/Topical Assignment 2/Assignment 02 Self Evaluation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B7A917-69A3-498D-9AC2-B855F7BA2ACE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701B8C34-95F4-47A1-8ECB-9D153463775B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="3645" windowWidth="18225" windowHeight="11423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 05" sheetId="1" r:id="rId1"/>
@@ -1729,18 +1729,6 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1762,6 +1750,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2080,8 +2080,8 @@
   <sheetPr codeName="shtAssignment05"/>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2102,15 +2102,15 @@
         <v>0</v>
       </c>
       <c r="C1" s="37"/>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="74" t="s">
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="73" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2121,14 +2121,14 @@
       </c>
       <c r="C2" s="38"/>
       <c r="D2" s="68">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="13"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="78"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="11"/>
@@ -2136,13 +2136,15 @@
         <v>10</v>
       </c>
       <c r="C3" s="38"/>
-      <c r="D3" s="68"/>
+      <c r="D3" s="68">
+        <v>2</v>
+      </c>
       <c r="E3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="78"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="11"/>
@@ -2155,8 +2157,8 @@
         <v>5</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="79"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="75"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="11"/>
@@ -2208,7 +2210,7 @@
       <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="76" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -2229,7 +2231,7 @@
       <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" s="70"/>
+      <c r="A9" s="77"/>
       <c r="B9" s="12" t="s">
         <v>17</v>
       </c>
@@ -2250,7 +2252,7 @@
       <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="70"/>
+      <c r="A10" s="77"/>
       <c r="B10" s="12" t="s">
         <v>107</v>
       </c>
@@ -2271,7 +2273,7 @@
       <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" s="70"/>
+      <c r="A11" s="77"/>
       <c r="B11" s="12" t="s">
         <v>18</v>
       </c>
@@ -2292,7 +2294,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="72"/>
+      <c r="A12" s="78"/>
       <c r="B12" s="12" t="s">
         <v>19</v>
       </c>
@@ -2313,7 +2315,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="79" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="25" t="s">
@@ -2336,7 +2338,7 @@
       <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="70"/>
+      <c r="A14" s="77"/>
       <c r="B14" s="21" t="s">
         <v>33</v>
       </c>
@@ -2357,7 +2359,7 @@
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A15" s="70"/>
+      <c r="A15" s="77"/>
       <c r="B15" s="21" t="s">
         <v>59</v>
       </c>
@@ -2378,7 +2380,7 @@
       <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" s="70"/>
+      <c r="A16" s="77"/>
       <c r="B16" s="21" t="s">
         <v>61</v>
       </c>
@@ -2399,7 +2401,7 @@
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A17" s="70"/>
+      <c r="A17" s="77"/>
       <c r="B17" s="21" t="s">
         <v>47</v>
       </c>
@@ -2420,7 +2422,7 @@
       <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18" s="70"/>
+      <c r="A18" s="77"/>
       <c r="B18" s="21" t="s">
         <v>45</v>
       </c>
@@ -2441,7 +2443,7 @@
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" s="70"/>
+      <c r="A19" s="77"/>
       <c r="B19" s="21" t="s">
         <v>48</v>
       </c>
@@ -2462,7 +2464,7 @@
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A20" s="70"/>
+      <c r="A20" s="77"/>
       <c r="B20" s="21" t="s">
         <v>49</v>
       </c>
@@ -2483,7 +2485,7 @@
       <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A21" s="70"/>
+      <c r="A21" s="77"/>
       <c r="B21" s="21" t="s">
         <v>46</v>
       </c>
@@ -2504,7 +2506,7 @@
       <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A22" s="70"/>
+      <c r="A22" s="77"/>
       <c r="B22" s="21" t="s">
         <v>50</v>
       </c>
@@ -2525,7 +2527,7 @@
       <c r="H22" s="24"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A23" s="70"/>
+      <c r="A23" s="77"/>
       <c r="B23" s="21" t="s">
         <v>49</v>
       </c>
@@ -2546,7 +2548,7 @@
       <c r="H23" s="24"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A24" s="70"/>
+      <c r="A24" s="77"/>
       <c r="B24" s="21" t="s">
         <v>51</v>
       </c>
@@ -2567,7 +2569,7 @@
       <c r="H24" s="24"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A25" s="70"/>
+      <c r="A25" s="77"/>
       <c r="B25" s="21" t="s">
         <v>48</v>
       </c>
@@ -2588,7 +2590,7 @@
       <c r="H25" s="24"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A26" s="70"/>
+      <c r="A26" s="77"/>
       <c r="B26" s="21" t="s">
         <v>49</v>
       </c>
@@ -2609,7 +2611,7 @@
       <c r="H26" s="24"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A27" s="70"/>
+      <c r="A27" s="77"/>
       <c r="B27" s="21" t="s">
         <v>52</v>
       </c>
@@ -2630,7 +2632,7 @@
       <c r="H27" s="24"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A28" s="70"/>
+      <c r="A28" s="77"/>
       <c r="B28" s="21" t="s">
         <v>54</v>
       </c>
@@ -2651,7 +2653,7 @@
       <c r="H28" s="24"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" s="70"/>
+      <c r="A29" s="77"/>
       <c r="B29" s="21" t="s">
         <v>53</v>
       </c>
@@ -2672,7 +2674,7 @@
       <c r="H29" s="24"/>
     </row>
     <row r="30" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="72"/>
+      <c r="A30" s="78"/>
       <c r="B30" s="21" t="s">
         <v>64</v>
       </c>
@@ -2693,7 +2695,7 @@
       <c r="H30" s="24"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="79" t="s">
         <v>25</v>
       </c>
       <c r="B31" s="25" t="s">
@@ -2716,7 +2718,7 @@
       <c r="H31" s="20"/>
     </row>
     <row r="32" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A32" s="70"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="21" t="s">
         <v>55</v>
       </c>
@@ -2737,7 +2739,7 @@
       <c r="H32" s="24"/>
     </row>
     <row r="33" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A33" s="70"/>
+      <c r="A33" s="77"/>
       <c r="B33" s="21" t="s">
         <v>56</v>
       </c>
@@ -2758,7 +2760,7 @@
       <c r="H33" s="24"/>
     </row>
     <row r="34" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A34" s="70"/>
+      <c r="A34" s="77"/>
       <c r="B34" s="21" t="s">
         <v>57</v>
       </c>
@@ -2779,7 +2781,7 @@
       <c r="H34" s="24"/>
     </row>
     <row r="35" spans="1:8" ht="57" x14ac:dyDescent="0.45">
-      <c r="A35" s="70"/>
+      <c r="A35" s="77"/>
       <c r="B35" s="21" t="s">
         <v>58</v>
       </c>
@@ -2800,20 +2802,20 @@
       <c r="H35" s="24"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="70"/>
+      <c r="A36" s="77"/>
       <c r="B36" s="50" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="51"/>
       <c r="D36" s="52" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E36" s="53">
         <v>5</v>
       </c>
       <c r="F36" s="53">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G36" s="54"/>
       <c r="H36" s="54"/>
@@ -2830,13 +2832,13 @@
       <c r="E37" s="59"/>
       <c r="F37" s="59">
         <f>MAX(-35,SUM(F8:F36))</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G37" s="60"/>
       <c r="H37" s="60"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="71" t="s">
+      <c r="A38" s="76" t="s">
         <v>26</v>
       </c>
       <c r="B38" s="17" t="s">
@@ -2857,7 +2859,7 @@
       <c r="H38" s="20"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="70"/>
+      <c r="A39" s="77"/>
       <c r="B39" s="12" t="s">
         <v>17</v>
       </c>
@@ -2878,7 +2880,7 @@
       <c r="H39" s="16"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A40" s="70"/>
+      <c r="A40" s="77"/>
       <c r="B40" s="12" t="s">
         <v>107</v>
       </c>
@@ -2899,7 +2901,7 @@
       <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A41" s="70"/>
+      <c r="A41" s="77"/>
       <c r="B41" s="12" t="s">
         <v>18</v>
       </c>
@@ -2920,7 +2922,7 @@
       <c r="H41" s="16"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="72"/>
+      <c r="A42" s="78"/>
       <c r="B42" s="12" t="s">
         <v>19</v>
       </c>
@@ -2928,20 +2930,20 @@
         <v>16</v>
       </c>
       <c r="D42" s="48" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E42" s="49">
         <v>5</v>
       </c>
       <c r="F42" s="49">
         <f t="shared" si="6"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A43" s="69" t="s">
+      <c r="A43" s="79" t="s">
         <v>27</v>
       </c>
       <c r="B43" s="25" t="s">
@@ -2964,7 +2966,7 @@
       <c r="H43" s="28"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A44" s="70"/>
+      <c r="A44" s="77"/>
       <c r="B44" s="65" t="s">
         <v>83</v>
       </c>
@@ -2985,7 +2987,7 @@
       <c r="H44" s="67"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A45" s="70"/>
+      <c r="A45" s="77"/>
       <c r="B45" s="21" t="s">
         <v>42</v>
       </c>
@@ -3006,7 +3008,7 @@
       <c r="H45" s="24"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" s="70"/>
+      <c r="A46" s="77"/>
       <c r="B46" s="21" t="s">
         <v>71</v>
       </c>
@@ -3027,7 +3029,7 @@
       <c r="H46" s="24"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A47" s="70"/>
+      <c r="A47" s="77"/>
       <c r="B47" s="21" t="s">
         <v>74</v>
       </c>
@@ -3048,7 +3050,7 @@
       <c r="H47" s="24"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A48" s="70"/>
+      <c r="A48" s="77"/>
       <c r="B48" s="21" t="s">
         <v>75</v>
       </c>
@@ -3069,7 +3071,7 @@
       <c r="H48" s="24"/>
     </row>
     <row r="49" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A49" s="70"/>
+      <c r="A49" s="77"/>
       <c r="B49" s="21" t="s">
         <v>77</v>
       </c>
@@ -3090,7 +3092,7 @@
       <c r="H49" s="24"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A50" s="70"/>
+      <c r="A50" s="77"/>
       <c r="B50" s="21" t="s">
         <v>78</v>
       </c>
@@ -3111,7 +3113,7 @@
       <c r="H50" s="24"/>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="70"/>
+      <c r="A51" s="77"/>
       <c r="B51" s="50" t="s">
         <v>80</v>
       </c>
@@ -3143,13 +3145,13 @@
       <c r="E52" s="59"/>
       <c r="F52" s="59">
         <f>MAX(-30,SUM(F38:F51))</f>
-        <v>-8</v>
+        <v>-3</v>
       </c>
       <c r="G52" s="60"/>
       <c r="H52" s="60"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A53" s="71" t="s">
+      <c r="A53" s="76" t="s">
         <v>28</v>
       </c>
       <c r="B53" s="17" t="s">
@@ -3157,20 +3159,20 @@
       </c>
       <c r="C53" s="40"/>
       <c r="D53" s="18" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E53" s="19">
         <v>5</v>
       </c>
       <c r="F53" s="19">
         <f t="shared" ref="F53:F74" si="8">IF(D53="No",-E53,0)</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G53" s="20"/>
       <c r="H53" s="20"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A54" s="70"/>
+      <c r="A54" s="77"/>
       <c r="B54" s="12" t="s">
         <v>17</v>
       </c>
@@ -3178,20 +3180,20 @@
         <v>13</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E54" s="23">
         <v>5</v>
       </c>
       <c r="F54" s="23">
         <f t="shared" si="8"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G54" s="24"/>
       <c r="H54" s="16"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A55" s="70"/>
+      <c r="A55" s="77"/>
       <c r="B55" s="12" t="s">
         <v>107</v>
       </c>
@@ -3199,20 +3201,20 @@
         <v>14</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E55" s="23">
         <v>5</v>
       </c>
       <c r="F55" s="23">
         <f t="shared" si="8"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G55" s="24"/>
       <c r="H55" s="16"/>
     </row>
     <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="70"/>
+      <c r="A56" s="77"/>
       <c r="B56" s="12" t="s">
         <v>18</v>
       </c>
@@ -3220,20 +3222,20 @@
         <v>15</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E56" s="23">
         <v>5</v>
       </c>
       <c r="F56" s="23">
         <f t="shared" si="8"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G56" s="24"/>
       <c r="H56" s="16"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A57" s="72"/>
+      <c r="A57" s="78"/>
       <c r="B57" s="12" t="s">
         <v>19</v>
       </c>
@@ -3241,20 +3243,20 @@
         <v>16</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E57" s="49">
         <v>5</v>
       </c>
       <c r="F57" s="49">
         <f t="shared" si="8"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G57" s="16"/>
       <c r="H57" s="16"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A58" s="69" t="s">
+      <c r="A58" s="79" t="s">
         <v>29</v>
       </c>
       <c r="B58" s="25" t="s">
@@ -3277,7 +3279,7 @@
       <c r="H58" s="28"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A59" s="70"/>
+      <c r="A59" s="77"/>
       <c r="B59" s="65" t="s">
         <v>82</v>
       </c>
@@ -3285,20 +3287,20 @@
         <v>86</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E59" s="23">
         <v>3</v>
       </c>
       <c r="F59" s="23">
         <f t="shared" si="8"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G59" s="67"/>
       <c r="H59" s="67"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A60" s="70"/>
+      <c r="A60" s="77"/>
       <c r="B60" s="21" t="s">
         <v>84</v>
       </c>
@@ -3306,20 +3308,20 @@
         <v>85</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E60" s="23">
         <v>3</v>
       </c>
       <c r="F60" s="23">
         <f t="shared" ref="F60:F68" si="9">IF(D60="No",-E60,0)</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G60" s="24"/>
       <c r="H60" s="24"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A61" s="70"/>
+      <c r="A61" s="77"/>
       <c r="B61" s="64" t="s">
         <v>89</v>
       </c>
@@ -3340,7 +3342,7 @@
       <c r="H61" s="24"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A62" s="70"/>
+      <c r="A62" s="77"/>
       <c r="B62" s="64" t="s">
         <v>90</v>
       </c>
@@ -3361,7 +3363,7 @@
       <c r="H62" s="24"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A63" s="70"/>
+      <c r="A63" s="77"/>
       <c r="B63" s="21" t="s">
         <v>87</v>
       </c>
@@ -3382,7 +3384,7 @@
       <c r="H63" s="24"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A64" s="70"/>
+      <c r="A64" s="77"/>
       <c r="B64" s="21" t="s">
         <v>88</v>
       </c>
@@ -3403,7 +3405,7 @@
       <c r="H64" s="24"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A65" s="70"/>
+      <c r="A65" s="77"/>
       <c r="B65" s="21" t="s">
         <v>92</v>
       </c>
@@ -3424,7 +3426,7 @@
       <c r="H65" s="24"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A66" s="70"/>
+      <c r="A66" s="77"/>
       <c r="B66" s="21" t="s">
         <v>93</v>
       </c>
@@ -3445,7 +3447,7 @@
       <c r="H66" s="24"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A67" s="70"/>
+      <c r="A67" s="77"/>
       <c r="B67" s="21" t="s">
         <v>94</v>
       </c>
@@ -3466,7 +3468,7 @@
       <c r="H67" s="24"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A68" s="70"/>
+      <c r="A68" s="77"/>
       <c r="B68" s="64" t="s">
         <v>96</v>
       </c>
@@ -3487,7 +3489,7 @@
       <c r="H68" s="24"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A69" s="70"/>
+      <c r="A69" s="77"/>
       <c r="B69" s="64" t="s">
         <v>97</v>
       </c>
@@ -3508,7 +3510,7 @@
       <c r="H69" s="24"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A70" s="70"/>
+      <c r="A70" s="77"/>
       <c r="B70" s="21" t="s">
         <v>99</v>
       </c>
@@ -3529,7 +3531,7 @@
       <c r="H70" s="24"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A71" s="70"/>
+      <c r="A71" s="77"/>
       <c r="B71" s="21" t="s">
         <v>100</v>
       </c>
@@ -3550,7 +3552,7 @@
       <c r="H71" s="24"/>
     </row>
     <row r="72" spans="1:8" ht="57" x14ac:dyDescent="0.45">
-      <c r="A72" s="70"/>
+      <c r="A72" s="77"/>
       <c r="B72" s="21" t="s">
         <v>101</v>
       </c>
@@ -3571,7 +3573,7 @@
       <c r="H72" s="24"/>
     </row>
     <row r="73" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A73" s="70"/>
+      <c r="A73" s="77"/>
       <c r="B73" s="21" t="s">
         <v>102</v>
       </c>
@@ -3592,7 +3594,7 @@
       <c r="H73" s="24"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A74" s="70"/>
+      <c r="A74" s="77"/>
       <c r="B74" s="50" t="s">
         <v>104</v>
       </c>
@@ -3644,7 +3646,7 @@
       <c r="E77" s="63"/>
       <c r="F77" s="63">
         <f>MAX(-99,F7+F37+F52+F75)</f>
-        <v>-43</v>
+        <v>-33</v>
       </c>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
@@ -3659,7 +3661,7 @@
       <c r="E78" s="4"/>
       <c r="F78" s="4">
         <f>100+F77</f>
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="G78" s="6"/>
       <c r="H78" s="6"/>
@@ -3667,16 +3669,16 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="1Wy2qOxqzvlJZwC15VrqVUfgXri5CXyDLw8J9g9wUgLPNUERQeHFkBwl3BUP6E7QDvz410JUTtv4F78JJNxIXg==" saltValue="vMQlgNidT+i49dELMM/ijg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="10">
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A43:A51"/>
+    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="A58:A74"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:G4"/>
     <mergeCell ref="H1:H4"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A30"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A43:A51"/>
-    <mergeCell ref="A53:A57"/>
-    <mergeCell ref="A58:A74"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{0C4A7BFB-837E-4FE4-8988-52705A9B035E}">

</xml_diff>